<commit_message>
change student file structure
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>omda st</t>
   </si>
@@ -35,9 +35,6 @@
     <t>SPC</t>
   </si>
   <si>
-    <t>SPRG</t>
-  </si>
-  <si>
     <t>s-ahmeddakrory@zewailcity.edu.eg</t>
   </si>
   <si>
@@ -62,12 +59,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>completed credit hours</t>
-  </si>
-  <si>
-    <t>current credit hours</t>
-  </si>
-  <si>
     <t>GPA</t>
   </si>
   <si>
@@ -81,6 +72,21 @@
   </si>
   <si>
     <t>PEOPLE_ID</t>
+  </si>
+  <si>
+    <t>Earned Credit Hours</t>
+  </si>
+  <si>
+    <t>Registered Credit Hours</t>
+  </si>
+  <si>
+    <t>Attempted Credit hours</t>
+  </si>
+  <si>
+    <t>Transcipt</t>
+  </si>
+  <si>
+    <t>Fall</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,60 +427,69 @@
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
     <col min="12" max="12" width="24.5703125" customWidth="1"/>
     <col min="13" max="13" width="22.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
+      <c r="O1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>202000040</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1061690939</v>
@@ -492,7 +507,7 @@
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -505,6 +520,12 @@
       </c>
       <c r="M2" t="s">
         <v>0</v>
+      </c>
+      <c r="N2">
+        <v>66</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>